<commit_message>
update srs và phân công
</commit_message>
<xml_diff>
--- a/Phân công đánh giá công việc/PhanCongCongViecMoc1_2.xlsx
+++ b/Phân công đánh giá công việc/PhanCongCongViecMoc1_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\DACN_HeThongDatVe\Phân công đánh giá công việc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4DE0A90-3075-4EE2-B36C-D3EDB5DAC648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B55AFA2-DB9D-4A11-AFE0-5595236FD113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DE3126FE-7E61-4B77-B627-0259BC3103D7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="88">
   <si>
     <t>Mục tiêu</t>
   </si>
@@ -279,6 +279,30 @@
   </si>
   <si>
     <t>Xử lý chức năng chọn đồ ăn</t>
+  </si>
+  <si>
+    <t>Code giao diện và xử lý chức năng quản lí vé phim</t>
+  </si>
+  <si>
+    <t>Chức năng bán vé tại quầy???</t>
+  </si>
+  <si>
+    <t>Chức năng đổi mật khẩu???</t>
+  </si>
+  <si>
+    <t>Activity và Sequence chức năng quản lí phòng chiếu, lịch chiếu</t>
+  </si>
+  <si>
+    <t>MỐC 3: Tổng hợp tài liệu và xử lý các chức năng còn lại</t>
+  </si>
+  <si>
+    <t>Vẽ database</t>
+  </si>
+  <si>
+    <t>Thời gian còn lại</t>
+  </si>
+  <si>
+    <t>_ Hoàn thiện tài liệu SRS và thêm vài chức năng</t>
   </si>
 </sst>
 </file>
@@ -316,7 +340,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -362,6 +386,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -474,39 +504,72 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -516,41 +579,8 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -866,10 +896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B75F0CD7-5EDA-477E-B926-683C951ED0FC}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" topLeftCell="C39" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,20 +914,20 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -921,13 +951,13 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="21" t="s">
         <v>37</v>
       </c>
       <c r="D4" s="14" t="s">
@@ -941,9 +971,9 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A5" s="32"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="37"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="22"/>
       <c r="D5" s="8" t="s">
         <v>9</v>
       </c>
@@ -955,9 +985,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="32"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="37"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="22"/>
       <c r="D6" s="8" t="s">
         <v>16</v>
       </c>
@@ -969,9 +999,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A7" s="32"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="37"/>
+      <c r="A7" s="17"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="22"/>
       <c r="D7" s="8" t="s">
         <v>11</v>
       </c>
@@ -983,9 +1013,9 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A8" s="32"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="37"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="22"/>
       <c r="D8" s="11" t="s">
         <v>13</v>
       </c>
@@ -997,9 +1027,9 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A9" s="32"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="41"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="31"/>
       <c r="D9" s="15" t="s">
         <v>34</v>
       </c>
@@ -1011,11 +1041,11 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A10" s="32"/>
-      <c r="B10" s="17" t="s">
+      <c r="A10" s="17"/>
+      <c r="B10" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="C10" s="25" t="s">
         <v>36</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -1029,9 +1059,9 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A11" s="32"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="39"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="26"/>
       <c r="D11" s="7" t="s">
         <v>33</v>
       </c>
@@ -1043,9 +1073,9 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A12" s="32"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="39"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="26"/>
       <c r="D12" s="3" t="s">
         <v>32</v>
       </c>
@@ -1057,9 +1087,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A13" s="32"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="39"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="26"/>
       <c r="D13" s="3" t="s">
         <v>31</v>
       </c>
@@ -1071,9 +1101,9 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A14" s="32"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="39"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="26"/>
       <c r="D14" s="3" t="s">
         <v>35</v>
       </c>
@@ -1085,9 +1115,9 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A15" s="32"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="39"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="26"/>
       <c r="D15" s="3" t="s">
         <v>25</v>
       </c>
@@ -1099,11 +1129,11 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A16" s="32"/>
+      <c r="A16" s="17"/>
       <c r="B16" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="36" t="s">
+      <c r="C16" s="21" t="s">
         <v>28</v>
       </c>
       <c r="D16" s="8" t="s">
@@ -1117,9 +1147,9 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A17" s="32"/>
+      <c r="A17" s="17"/>
       <c r="B17" s="24"/>
-      <c r="C17" s="37"/>
+      <c r="C17" s="22"/>
       <c r="D17" s="8" t="s">
         <v>24</v>
       </c>
@@ -1131,9 +1161,9 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A18" s="32"/>
+      <c r="A18" s="17"/>
       <c r="B18" s="24"/>
-      <c r="C18" s="37"/>
+      <c r="C18" s="22"/>
       <c r="D18" s="8" t="s">
         <v>29</v>
       </c>
@@ -1145,9 +1175,9 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A19" s="32"/>
+      <c r="A19" s="17"/>
       <c r="B19" s="24"/>
-      <c r="C19" s="37"/>
+      <c r="C19" s="22"/>
       <c r="D19" s="8" t="s">
         <v>30</v>
       </c>
@@ -1159,9 +1189,9 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A20" s="32"/>
+      <c r="A20" s="17"/>
       <c r="B20" s="24"/>
-      <c r="C20" s="37"/>
+      <c r="C20" s="22"/>
       <c r="D20" s="8" t="s">
         <v>26</v>
       </c>
@@ -1173,9 +1203,9 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A21" s="32"/>
+      <c r="A21" s="17"/>
       <c r="B21" s="24"/>
-      <c r="C21" s="37"/>
+      <c r="C21" s="22"/>
       <c r="D21" s="8" t="s">
         <v>68</v>
       </c>
@@ -1187,11 +1217,11 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="32"/>
-      <c r="B22" s="17" t="s">
+      <c r="A22" s="17"/>
+      <c r="B22" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="38" t="s">
+      <c r="C22" s="25" t="s">
         <v>40</v>
       </c>
       <c r="D22" s="3" t="s">
@@ -1205,9 +1235,9 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="32"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="39"/>
+      <c r="A23" s="17"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="26"/>
       <c r="D23" s="3" t="s">
         <v>70</v>
       </c>
@@ -1219,9 +1249,9 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A24" s="32"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="39"/>
+      <c r="A24" s="17"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="26"/>
       <c r="D24" s="3" t="s">
         <v>39</v>
       </c>
@@ -1233,9 +1263,9 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A25" s="32"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="39"/>
+      <c r="A25" s="17"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="26"/>
       <c r="D25" s="3" t="s">
         <v>27</v>
       </c>
@@ -1247,9 +1277,9 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A26" s="33"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="40"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="27"/>
       <c r="D26" s="6" t="s">
         <v>47</v>
       </c>
@@ -1261,13 +1291,13 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="35" t="s">
         <v>61</v>
       </c>
       <c r="B27" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="25" t="s">
+      <c r="C27" s="32" t="s">
         <v>55</v>
       </c>
       <c r="D27" s="8" t="s">
@@ -1281,9 +1311,9 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="16"/>
+      <c r="A28" s="35"/>
       <c r="B28" s="24"/>
-      <c r="C28" s="26"/>
+      <c r="C28" s="33"/>
       <c r="D28" s="8" t="s">
         <v>42</v>
       </c>
@@ -1295,9 +1325,9 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A29" s="16"/>
+      <c r="A29" s="35"/>
       <c r="B29" s="24"/>
-      <c r="C29" s="26"/>
+      <c r="C29" s="33"/>
       <c r="D29" s="8" t="s">
         <v>43</v>
       </c>
@@ -1309,9 +1339,9 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A30" s="16"/>
-      <c r="B30" s="29"/>
-      <c r="C30" s="30"/>
+      <c r="A30" s="35"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="34"/>
       <c r="D30" s="11" t="s">
         <v>44</v>
       </c>
@@ -1323,11 +1353,11 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A31" s="16"/>
-      <c r="B31" s="17" t="s">
+      <c r="A31" s="35"/>
+      <c r="B31" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="20" t="s">
+      <c r="C31" s="36" t="s">
         <v>49</v>
       </c>
       <c r="D31" s="3" t="s">
@@ -1341,9 +1371,9 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A32" s="16"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="21"/>
+      <c r="A32" s="35"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="37"/>
       <c r="D32" s="3" t="s">
         <v>72</v>
       </c>
@@ -1355,9 +1385,9 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A33" s="16"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="21"/>
+      <c r="A33" s="35"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="37"/>
       <c r="D33" s="3" t="s">
         <v>71</v>
       </c>
@@ -1369,9 +1399,9 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A34" s="16"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="21"/>
+      <c r="A34" s="35"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="37"/>
       <c r="D34" s="3" t="s">
         <v>73</v>
       </c>
@@ -1383,219 +1413,297 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A35" s="16"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="21"/>
+      <c r="A35" s="35"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="37"/>
       <c r="D35" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A36" s="35"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="37"/>
+      <c r="D36" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A37" s="35"/>
+      <c r="B37" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F37" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A38" s="35"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="33"/>
+      <c r="D38" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F38" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A39" s="35"/>
+      <c r="B39" s="24"/>
+      <c r="C39" s="33"/>
+      <c r="D39" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A40" s="35"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F40" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A41" s="35"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="33"/>
+      <c r="D41" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A42" s="35"/>
+      <c r="B42" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="C42" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A43" s="35"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="39"/>
+      <c r="D43" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F43" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A44" s="35"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="39"/>
+      <c r="D44" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F44" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A45" s="35"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="39"/>
+      <c r="D45" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E45" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F35" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A36" s="16"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F36" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A37" s="16"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F37" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A38" s="16"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F38" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A39" s="16"/>
-      <c r="B39" s="19"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F39" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A40" s="16"/>
-      <c r="B40" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="C40" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="E40" s="10" t="s">
+      <c r="F45" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A46" s="35"/>
+      <c r="B46" s="38"/>
+      <c r="C46" s="39"/>
+      <c r="D46" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E46" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F40" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A41" s="16"/>
-      <c r="B41" s="24"/>
-      <c r="C41" s="26"/>
-      <c r="D41" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="E41" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F41" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A42" s="16"/>
-      <c r="B42" s="24"/>
-      <c r="C42" s="26"/>
-      <c r="D42" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F42" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A43" s="16"/>
-      <c r="B43" s="24"/>
-      <c r="C43" s="26"/>
-      <c r="D43" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F43" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A44" s="16"/>
-      <c r="B44" s="24"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="11" t="s">
+      <c r="F46" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="B47" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="C47" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="D47" s="11" t="s">
         <v>79</v>
-      </c>
-      <c r="E44" s="9"/>
-      <c r="F44" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A45" s="16"/>
-      <c r="B45" s="24"/>
-      <c r="C45" s="26"/>
-      <c r="D45" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="E45" s="9"/>
-      <c r="F45" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A46" s="16"/>
-      <c r="B46" s="24"/>
-      <c r="C46" s="26"/>
-      <c r="D46" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E46" s="9"/>
-      <c r="F46" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A47" s="16"/>
-      <c r="B47" s="24"/>
-      <c r="C47" s="26"/>
-      <c r="D47" s="8" t="s">
-        <v>76</v>
       </c>
       <c r="E47" s="9"/>
       <c r="F47" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A48" s="16"/>
-      <c r="B48" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="C48" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E48" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F48" s="13" t="s">
-        <v>5</v>
+    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="41"/>
+      <c r="B48" s="24"/>
+      <c r="C48" s="33"/>
+      <c r="D48" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E48" s="9"/>
+      <c r="F48" s="5" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A49" s="16"/>
-      <c r="B49" s="27"/>
-      <c r="C49" s="28"/>
-      <c r="D49" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="A49" s="41"/>
+      <c r="B49" s="24"/>
+      <c r="C49" s="33"/>
+      <c r="D49" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E49" s="9"/>
       <c r="F49" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A50" s="41"/>
+      <c r="B50" s="24"/>
+      <c r="C50" s="33"/>
+      <c r="D50" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E50" s="9"/>
+      <c r="F50" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A51" s="41"/>
+      <c r="B51" s="24"/>
+      <c r="C51" s="33"/>
+      <c r="D51" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E51" s="10"/>
+      <c r="F51" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A52" s="41"/>
+      <c r="B52" s="24"/>
+      <c r="C52" s="33"/>
+      <c r="D52" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E52" s="10"/>
+      <c r="F52" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A53" s="41"/>
+      <c r="B53" s="24"/>
+      <c r="C53" s="33"/>
+      <c r="D53" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E53" s="10"/>
+      <c r="F53" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A54" s="41"/>
+      <c r="B54" s="24"/>
+      <c r="C54" s="33"/>
+      <c r="D54" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E54" s="10"/>
+      <c r="F54" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="22">
+    <mergeCell ref="A47:A54"/>
+    <mergeCell ref="B47:B54"/>
+    <mergeCell ref="C47:C54"/>
+    <mergeCell ref="A27:A46"/>
+    <mergeCell ref="B31:B36"/>
+    <mergeCell ref="C31:C36"/>
+    <mergeCell ref="B37:B41"/>
+    <mergeCell ref="C37:C41"/>
+    <mergeCell ref="B42:B46"/>
+    <mergeCell ref="C42:C46"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
     <mergeCell ref="A4:A26"/>
     <mergeCell ref="B1:E2"/>
     <mergeCell ref="C16:C21"/>
@@ -1606,15 +1714,6 @@
     <mergeCell ref="B4:B9"/>
     <mergeCell ref="C10:C15"/>
     <mergeCell ref="B10:B15"/>
-    <mergeCell ref="A27:A49"/>
-    <mergeCell ref="B31:B39"/>
-    <mergeCell ref="C31:C39"/>
-    <mergeCell ref="B40:B47"/>
-    <mergeCell ref="C40:C47"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Xử lý chức năng mua đồ ăn và giỏ hàng
</commit_message>
<xml_diff>
--- a/Phân công đánh giá công việc/PhanCongCongViecMoc1_2.xlsx
+++ b/Phân công đánh giá công việc/PhanCongCongViecMoc1_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\DACN_HeThongDatVe\Phân công đánh giá công việc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{285A6A93-6F25-49FF-A055-88C7D590CF79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E69E6B2-C225-480B-BB9F-A2C95DC1E41B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DE3126FE-7E61-4B77-B627-0259BC3103D7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="88">
   <si>
     <t>Mục tiêu</t>
   </si>
@@ -278,9 +278,6 @@
     <t>Code giao diện và xử lý chức năng quản lí vé phim</t>
   </si>
   <si>
-    <t>Chức năng bán vé tại quầy???</t>
-  </si>
-  <si>
     <t>Chức năng đổi mật khẩu???</t>
   </si>
   <si>
@@ -303,6 +300,9 @@
   </si>
   <si>
     <t>_Code xử lý các chức năng quản lí thông tin nhân viên và khách hàng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sửa chức năng đăng kí </t>
   </si>
 </sst>
 </file>
@@ -898,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B75F0CD7-5EDA-477E-B926-683C951ED0FC}">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D39" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" topLeftCell="D40" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1292,7 +1292,7 @@
     </row>
     <row r="27" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B27" s="17" t="s">
         <v>45</v>
@@ -1446,7 +1446,7 @@
         <v>64</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D37" s="11" t="s">
         <v>75</v>
@@ -1590,18 +1590,20 @@
     </row>
     <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B47" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C47" s="19" t="s">
         <v>84</v>
-      </c>
-      <c r="C47" s="19" t="s">
-        <v>85</v>
       </c>
       <c r="D47" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="E47" s="9"/>
+      <c r="E47" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="F47" s="5" t="s">
         <v>60</v>
       </c>
@@ -1613,7 +1615,9 @@
       <c r="D48" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="E48" s="9"/>
+      <c r="E48" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="F48" s="5" t="s">
         <v>60</v>
       </c>
@@ -1625,9 +1629,11 @@
       <c r="D49" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E49" s="9"/>
-      <c r="F49" s="5" t="s">
-        <v>60</v>
+      <c r="E49" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F49" s="13" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -1640,8 +1646,8 @@
       <c r="E50" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F50" s="5" t="s">
-        <v>60</v>
+      <c r="F50" s="13" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -1649,9 +1655,11 @@
       <c r="B51" s="18"/>
       <c r="C51" s="20"/>
       <c r="D51" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="E51" s="10"/>
+        <v>80</v>
+      </c>
+      <c r="E51" s="9" t="s">
+        <v>12</v>
+      </c>
       <c r="F51" s="5" t="s">
         <v>60</v>
       </c>
@@ -1661,13 +1669,13 @@
       <c r="B52" s="18"/>
       <c r="C52" s="20"/>
       <c r="D52" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E52" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F52" s="5" t="s">
-        <v>60</v>
+      <c r="F52" s="13" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -1675,9 +1683,11 @@
       <c r="B53" s="18"/>
       <c r="C53" s="20"/>
       <c r="D53" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="E53" s="10"/>
+        <v>87</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="F53" s="5" t="s">
         <v>60</v>
       </c>
@@ -1687,9 +1697,11 @@
       <c r="B54" s="18"/>
       <c r="C54" s="20"/>
       <c r="D54" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="E54" s="10"/>
+        <v>82</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>12</v>
+      </c>
       <c r="F54" s="5" t="s">
         <v>60</v>
       </c>

</xml_diff>